<commit_message>
Correction du cours 7
</commit_message>
<xml_diff>
--- a/M1_Finance_Cours_7.xlsx
+++ b/M1_Finance_Cours_7.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amtti\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amtti\Documents\Université\Finance\M1_Finance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9857D9E-758C-47D6-A06D-970ED3FF2774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC684547-5E3F-4C19-8FBD-B8DB7EDA724D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{CEAE8C27-10B7-480F-8270-3D6E34E88447}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="62">
   <si>
     <t>RES EXPL ordinaire hors DAP</t>
   </si>
@@ -172,7 +172,58 @@
     <t>5ième année 119ième jour</t>
   </si>
   <si>
-    <t>5ième année 330ième jour</t>
+    <t>VANG</t>
+  </si>
+  <si>
+    <t>TRIG</t>
+  </si>
+  <si>
+    <t>Correction</t>
+  </si>
+  <si>
+    <t>Dans ce genre de cas, la solution dépend de ce que veulent les associés, la direction.</t>
+  </si>
+  <si>
+    <t>Les deux projets rapportent plus de 6% (norme marchés financiers) avec des revenus réguliers là où les marchés financiers ne rapportent les 6% qu'au bout de 5 ans.</t>
+  </si>
+  <si>
+    <t>DRCI</t>
+  </si>
+  <si>
+    <t>ERC</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Actualisés cummulés</t>
+  </si>
+  <si>
+    <t>Vrai TRR</t>
+  </si>
+  <si>
+    <t>Ensuite il faut trouver quelque chose dans l'ordre de 25% avec un calcul que je n'ai pas encore compris.</t>
+  </si>
+  <si>
+    <t>Le TRR est le taux de rendement du capital investi. Le taux qui annule le capital investi supplémentaire.</t>
+  </si>
+  <si>
+    <t>Ici, nos 470 millions supplémentaires rapportent 25% de plus à eux seuls.</t>
+  </si>
+  <si>
+    <t>6ième année 129ième jour</t>
+  </si>
+  <si>
+    <t>Mai</t>
+  </si>
+  <si>
+    <t>9 Mai N+6</t>
+  </si>
+  <si>
+    <t>Actualisés</t>
   </si>
 </sst>
 </file>
@@ -225,11 +276,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -239,10 +291,12 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Milliers" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Pourcentage" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1056,10 +1110,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A43CF8A4-2CCC-48AC-93C1-E83ED2E3724D}">
-  <dimension ref="A1:L49"/>
+  <dimension ref="A1:L66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1067,7 +1121,9 @@
     <col min="1" max="1" width="17.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="12" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
@@ -1219,94 +1275,163 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="C16" s="8">
-        <f>SUM($C$15:C15)</f>
-        <v>204000000</v>
-      </c>
-      <c r="D16" s="8">
-        <f>SUM($C$15:D15)</f>
-        <v>408000000</v>
-      </c>
-      <c r="E16" s="8">
-        <f>SUM($C$15:E15)</f>
-        <v>612000000</v>
-      </c>
-      <c r="F16" s="8">
-        <f>SUM($C$15:F15)</f>
-        <v>816000000</v>
-      </c>
-      <c r="G16" s="8">
-        <f>SUM($C$15:G15)</f>
-        <v>1020000000</v>
-      </c>
-      <c r="H16" s="8">
-        <f>SUM($C$15:H15)</f>
-        <v>1224000000</v>
-      </c>
-      <c r="I16" s="8">
-        <f>SUM($C$15:I15)</f>
-        <v>1428000000</v>
-      </c>
-      <c r="J16" s="8">
-        <f>SUM($C$15:J15)</f>
-        <v>1632000000</v>
-      </c>
-      <c r="K16" s="8">
-        <f>SUM($C$15:K15)</f>
-        <v>1836000000</v>
-      </c>
-      <c r="L16" s="8">
-        <f>SUM($C$15:L15)</f>
-        <v>2040000000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F17" s="3">
-        <f>-B15-F16</f>
-        <v>184000000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="3">
+        <f>C15*(0.93^C14)</f>
+        <v>189720000</v>
+      </c>
+      <c r="D16" s="3">
+        <f>D15*(0.93^D14)</f>
+        <v>176439600.00000003</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" ref="E16:L16" si="2">E15*(0.93^E14)</f>
+        <v>164088828.00000003</v>
+      </c>
+      <c r="F16" s="3">
+        <f t="shared" si="2"/>
+        <v>152602610.04000005</v>
+      </c>
+      <c r="G16" s="3">
+        <f t="shared" si="2"/>
+        <v>141920427.33720005</v>
+      </c>
+      <c r="H16" s="3">
+        <f t="shared" si="2"/>
+        <v>131985997.42359605</v>
+      </c>
+      <c r="I16" s="3">
+        <f t="shared" si="2"/>
+        <v>122746977.60394433</v>
+      </c>
+      <c r="J16" s="3">
+        <f t="shared" si="2"/>
+        <v>114154689.17166825</v>
+      </c>
+      <c r="K16" s="3">
+        <f t="shared" si="2"/>
+        <v>106163860.92965147</v>
+      </c>
+      <c r="L16" s="3">
+        <f t="shared" si="2"/>
+        <v>98732390.664575875</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="8">
+        <f>SUM($C$16:C16)</f>
+        <v>189720000</v>
+      </c>
+      <c r="D17" s="8">
+        <f>SUM($C$16:D16)</f>
+        <v>366159600</v>
+      </c>
+      <c r="E17" s="8">
+        <f>SUM($C$16:E16)</f>
+        <v>530248428</v>
+      </c>
+      <c r="F17" s="8">
+        <f>SUM($C$16:F16)</f>
+        <v>682851038.04000008</v>
+      </c>
+      <c r="G17" s="8">
+        <f>SUM($C$16:G16)</f>
+        <v>824771465.37720013</v>
+      </c>
+      <c r="H17" s="8">
+        <f>SUM($C$16:H16)</f>
+        <v>956757462.80079615</v>
+      </c>
+      <c r="I17" s="8">
+        <f>SUM($C$16:I16)</f>
+        <v>1079504440.4047406</v>
+      </c>
+      <c r="J17" s="8">
+        <f>SUM($C$16:J16)</f>
+        <v>1193659129.5764089</v>
+      </c>
+      <c r="K17" s="8">
+        <f>SUM($C$16:K16)</f>
+        <v>1299822990.5060604</v>
+      </c>
+      <c r="L17" s="8">
+        <f>SUM($C$16:L16)</f>
+        <v>1398555381.1706362</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F18" s="3">
+        <f>-B15-H17</f>
+        <v>43242537.199203849</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B19" s="4">
         <f>NPV(C3,C15:L15)+B15</f>
         <v>432810634.35025048</v>
       </c>
-      <c r="F18" s="3">
-        <f>G16-F16</f>
-        <v>204000000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="F19" s="3">
+        <f>I17-H17</f>
+        <v>122746977.60394442</v>
+      </c>
+      <c r="G19" s="3"/>
+      <c r="I19" s="3">
+        <f>-B15-H17</f>
+        <v>43242537.199203849</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B20" s="6">
         <f>IRR(B15:L15)</f>
         <v>0.15622389078164378</v>
       </c>
-      <c r="F19">
-        <f>F17/F18</f>
-        <v>0.90196078431372551</v>
-      </c>
-      <c r="G19">
-        <f>F19*365</f>
-        <v>329.21568627450984</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G20" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F20" s="9">
+        <f>F18/F19</f>
+        <v>0.35229003632765837</v>
+      </c>
+      <c r="G20">
+        <f>F20*365</f>
+        <v>128.5858632595953</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G22">
+        <f>G20/30</f>
+        <v>4.2861954419865098</v>
+      </c>
+      <c r="H22" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G23">
+        <f>(G22-4)*30</f>
+        <v>8.5858632595952944</v>
+      </c>
+      <c r="H23">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1316,8 +1441,11 @@
       <c r="D25">
         <v>500000</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H25" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -1328,7 +1456,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -1339,7 +1467,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>37</v>
       </c>
@@ -1352,7 +1480,7 @@
         <v>340000000</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -1361,7 +1489,7 @@
         <v>1900</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -1370,7 +1498,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -1400,35 +1528,35 @@
         <v>2</v>
       </c>
       <c r="E37">
-        <f t="shared" ref="E37" si="2">D37+1</f>
+        <f t="shared" ref="E37" si="3">D37+1</f>
         <v>3</v>
       </c>
       <c r="F37">
-        <f t="shared" ref="F37" si="3">E37+1</f>
+        <f t="shared" ref="F37" si="4">E37+1</f>
         <v>4</v>
       </c>
       <c r="G37">
-        <f t="shared" ref="G37" si="4">F37+1</f>
+        <f t="shared" ref="G37" si="5">F37+1</f>
         <v>5</v>
       </c>
       <c r="H37">
-        <f t="shared" ref="H37" si="5">G37+1</f>
+        <f t="shared" ref="H37" si="6">G37+1</f>
         <v>6</v>
       </c>
       <c r="I37">
-        <f t="shared" ref="I37" si="6">H37+1</f>
+        <f t="shared" ref="I37" si="7">H37+1</f>
         <v>7</v>
       </c>
       <c r="J37">
-        <f t="shared" ref="J37" si="7">I37+1</f>
+        <f t="shared" ref="J37" si="8">I37+1</f>
         <v>8</v>
       </c>
       <c r="K37">
-        <f t="shared" ref="K37" si="8">J37+1</f>
+        <f t="shared" ref="K37" si="9">J37+1</f>
         <v>9</v>
       </c>
       <c r="L37">
-        <f t="shared" ref="L37" si="9">K37+1</f>
+        <f t="shared" ref="L37" si="10">K37+1</f>
         <v>10</v>
       </c>
     </row>
@@ -1444,143 +1572,298 @@
         <v>340000000</v>
       </c>
       <c r="D38" s="3">
-        <f t="shared" ref="D38:L38" si="10">$B$33</f>
+        <f t="shared" ref="D38:L38" si="11">$B$33</f>
         <v>340000000</v>
       </c>
       <c r="E38" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>340000000</v>
       </c>
       <c r="F38" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>340000000</v>
       </c>
       <c r="G38" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>340000000</v>
       </c>
       <c r="H38" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>340000000</v>
       </c>
       <c r="I38" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>340000000</v>
       </c>
       <c r="J38" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>340000000</v>
       </c>
       <c r="K38" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>340000000</v>
       </c>
       <c r="L38" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>340000000</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>61</v>
+      </c>
+      <c r="C39" s="3">
+        <f>C38*(0.93^C37)</f>
+        <v>316200000</v>
+      </c>
+      <c r="D39" s="3">
+        <f t="shared" ref="D39:L39" si="12">D38*(0.93^D37)</f>
+        <v>294066000.00000006</v>
+      </c>
+      <c r="E39" s="3">
+        <f t="shared" si="12"/>
+        <v>273481380.00000006</v>
+      </c>
+      <c r="F39" s="3">
+        <f t="shared" si="12"/>
+        <v>254337683.40000007</v>
+      </c>
+      <c r="G39" s="3">
+        <f t="shared" si="12"/>
+        <v>236534045.56200007</v>
+      </c>
+      <c r="H39" s="3">
+        <f t="shared" si="12"/>
+        <v>219976662.3726601</v>
+      </c>
+      <c r="I39" s="3">
+        <f t="shared" si="12"/>
+        <v>204578296.00657389</v>
+      </c>
+      <c r="J39" s="3">
+        <f t="shared" si="12"/>
+        <v>190257815.28611377</v>
+      </c>
+      <c r="K39" s="3">
+        <f t="shared" si="12"/>
+        <v>176939768.21608579</v>
+      </c>
+      <c r="L39" s="3">
+        <f t="shared" si="12"/>
+        <v>164553984.44095981</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>10</v>
       </c>
-      <c r="C39" s="8">
+      <c r="C40" s="8">
         <f>SUM($C$38:C38)</f>
         <v>340000000</v>
       </c>
-      <c r="D39" s="8">
+      <c r="D40" s="8">
         <f>SUM($C$38:D38)</f>
         <v>680000000</v>
       </c>
-      <c r="E39" s="8">
+      <c r="E40" s="8">
         <f>SUM($C$38:E38)</f>
         <v>1020000000</v>
       </c>
-      <c r="F39" s="8">
+      <c r="F40" s="8">
         <f>SUM($C$38:F38)</f>
         <v>1360000000</v>
       </c>
-      <c r="G39" s="8">
+      <c r="G40" s="8">
         <f>SUM($C$38:G38)</f>
         <v>1700000000</v>
       </c>
-      <c r="H39" s="8">
+      <c r="H40" s="8">
         <f>SUM($C$38:H38)</f>
         <v>2040000000</v>
       </c>
-      <c r="I39" s="8">
+      <c r="I40" s="8">
         <f>SUM($C$38:I38)</f>
         <v>2380000000</v>
       </c>
-      <c r="J39" s="8">
+      <c r="J40" s="8">
         <f>SUM($C$38:J38)</f>
         <v>2720000000</v>
       </c>
-      <c r="K39" s="8">
+      <c r="K40" s="8">
         <f>SUM($C$38:K38)</f>
         <v>3060000000</v>
       </c>
-      <c r="L39" s="8">
+      <c r="L40" s="8">
         <f>SUM($C$38:L38)</f>
         <v>3400000000</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="F40" s="3">
-        <f>-B38-F39</f>
-        <v>110000000</v>
-      </c>
-    </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F41" s="3">
-        <f>G39-F39</f>
+        <f>-B38-F40</f>
+        <v>110000000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F42" s="3">
+        <f>G40-F40</f>
         <v>340000000</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="F42">
-        <f>F40/F41</f>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F43">
+        <f>F41/F42</f>
         <v>0.3235294117647059</v>
       </c>
-      <c r="G42" s="7">
-        <f>F42*365</f>
+      <c r="G43" s="7">
+        <f>F43*365</f>
         <v>118.08823529411765</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>30</v>
       </c>
-      <c r="B43" s="4">
+      <c r="B44" s="4">
         <f>NPV(C3,C38:L38)+B38</f>
         <v>918017723.91708374</v>
       </c>
-      <c r="G43" t="s">
+      <c r="G44" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
         <v>34</v>
       </c>
-      <c r="B44" s="6">
+      <c r="B45" s="6">
         <f>IRR(B38:L38)</f>
         <v>0.1910252863313302</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>36</v>
       </c>
-      <c r="B48" s="4">
-        <f>B43-B18</f>
+      <c r="B49" s="4">
+        <f>B44-B19</f>
         <v>485207089.56683326</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B49" s="6">
-        <f>B44-B19</f>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B50" s="6">
+        <f>B45-B20</f>
         <v>3.480139554968642E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>22</v>
+      </c>
+      <c r="C54" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>30</v>
+      </c>
+      <c r="B55" s="4">
+        <f>B19</f>
+        <v>432810634.35025048</v>
+      </c>
+      <c r="C55" s="4">
+        <f>B44</f>
+        <v>918017723.91708374</v>
+      </c>
+      <c r="D55" t="s">
+        <v>51</v>
+      </c>
+      <c r="E55" s="4">
+        <f>C55-B55</f>
+        <v>485207089.56683326</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>34</v>
+      </c>
+      <c r="B56" s="6">
+        <f>B20</f>
+        <v>0.15622389078164378</v>
+      </c>
+      <c r="C56" s="6">
+        <f>B45</f>
+        <v>0.1910252863313302</v>
+      </c>
+      <c r="D56" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>49</v>
+      </c>
+      <c r="B57">
+        <f>G20</f>
+        <v>128.5858632595953</v>
+      </c>
+      <c r="C57" s="7">
+        <f>G43</f>
+        <v>118.08823529411765</v>
+      </c>
+      <c r="D57" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>50</v>
+      </c>
+      <c r="B58" s="9">
+        <f>1+B55/B15</f>
+        <v>0.56718936564974953</v>
+      </c>
+      <c r="C58" s="9">
+        <f>1+C55/B38</f>
+        <v>0.37549814699518114</v>
+      </c>
+      <c r="D58" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F60" s="3">
+        <f>C38-C15</f>
+        <v>136000000</v>
+      </c>
+      <c r="G60" s="3">
+        <f>B15-B38</f>
+        <v>470000000</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>54</v>
+      </c>
+      <c r="B63">
+        <f>G60/F60</f>
+        <v>3.4558823529411766</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B64" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B65" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B66" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1590,10 +1873,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80A53A76-E188-42B7-9BAE-8F499DEFB9AE}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1601,20 +1884,23 @@
     <col min="1" max="1" width="16.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="2">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -1639,8 +1925,14 @@
       <c r="H3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1667,8 +1959,14 @@
         <f>IRR(B4:F4)</f>
         <v>7.4969819653015524E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4">
+        <v>8.42</v>
+      </c>
+      <c r="J4" s="6">
+        <v>7.1400000000000005E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -1695,8 +1993,14 @@
         <f>IRR(B5:F5)</f>
         <v>8.9843285136826712E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5">
+        <v>8.6</v>
+      </c>
+      <c r="J5" s="6">
+        <v>7.1800000000000003E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -1724,9 +2028,19 @@
         <v>26.247696000000005</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B8" s="2">
         <v>0.06</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>